<commit_message>
adjustments to the appendix and addition of C5 and C6
</commit_message>
<xml_diff>
--- a/Tables/SupplementalTable2.xlsx
+++ b/Tables/SupplementalTable2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="22460" yWindow="0" windowWidth="25600" windowHeight="19660" tabRatio="500"/>
@@ -89,7 +89,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -112,6 +112,22 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -219,14 +235,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -236,24 +267,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -586,17 +606,17 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="5"/>
-    <col min="2" max="2" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="34" customHeight="1" thickBot="1">
@@ -610,102 +630,102 @@
       <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" ht="16" thickBot="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" ht="16" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" thickBot="1">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="7" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" ht="16" thickBot="1">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="7" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="7" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" thickBot="1">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="7" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" thickBot="1">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="7" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16" thickBot="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="7" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -716,6 +736,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>